<commit_message>
Novas melhorias e adicoes ao codigo
</commit_message>
<xml_diff>
--- a/src/test/resources/excelUtil/paginaUsuario.xlsx
+++ b/src/test/resources/excelUtil/paginaUsuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.corticeiro\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269E6421-8BFB-4A2A-A117-33B4DEBFFB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52976E0-4225-4516-8659-8A7BEACF9BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2115" yWindow="960" windowWidth="17610" windowHeight="7875" xr2:uid="{3ECD08F1-08EC-4C21-A4FD-A3D2BD600672}"/>
   </bookViews>
@@ -102,7 +102,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Teste14</t>
+    <t>Testee05</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
arrumadno o nome das steps
</commit_message>
<xml_diff>
--- a/src/test/resources/excelUtil/paginaUsuario.xlsx
+++ b/src/test/resources/excelUtil/paginaUsuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.corticeiro\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C7194A-DE48-4B23-86E3-E879ECFB196B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5780599E-F057-433D-A6A1-CB5FA2747269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1035" windowWidth="17610" windowHeight="7875" xr2:uid="{3ECD08F1-08EC-4C21-A4FD-A3D2BD600672}"/>
   </bookViews>
@@ -102,7 +102,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>tesTe01</t>
+    <t>tesTe02</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding reports with screenshots
</commit_message>
<xml_diff>
--- a/src/test/resources/excelUtil/paginaUsuario.xlsx
+++ b/src/test/resources/excelUtil/paginaUsuario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.corticeiro\eclipse-workspace\AdvantageTestes\src\test\resources\excelUtil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2150F2-8196-42D2-933E-1A44FD168594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083F452C-4E20-4302-9E54-05D82DDC9046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-150" yWindow="1140" windowWidth="17610" windowHeight="7875" xr2:uid="{3ECD08F1-08EC-4C21-A4FD-A3D2BD600672}"/>
+    <workbookView xWindow="2535" yWindow="1065" windowWidth="17610" windowHeight="7875" xr2:uid="{3ECD08F1-08EC-4C21-A4FD-A3D2BD600672}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroUsuario" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>tesTe07</t>
+    <t>tesTe08</t>
   </si>
 </sst>
 </file>

</xml_diff>